<commit_message>
[REPO] Correcciones código inflación mas tablas datawrapper
</commit_message>
<xml_diff>
--- a/01_datos_crudos/01_03_inpc_complete_NewVersion.xlsx
+++ b/01_datos_crudos/01_03_inpc_complete_NewVersion.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sam/Documents/GitHub/mcv_inflacion/01_datos_crudos/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jorgejuvenalcamposferreira/Documents/GitHub/mcv_inflacion/01_datos_crudos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C26C5585-2953-FF44-9226-3261248404D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E12E3D7-AFCE-E442-AE3C-2E62779D3E60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12300" yWindow="640" windowWidth="16500" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="46820" yWindow="500" windowWidth="16500" windowHeight="17020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3826" uniqueCount="2175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3825" uniqueCount="2174">
   <si>
     <t>ccif</t>
   </si>
@@ -6294,9 +6294,6 @@
   </si>
   <si>
     <t>909068</t>
-  </si>
-  <si>
-    <t>909069</t>
   </si>
   <si>
     <t>909070</t>
@@ -7040,8 +7037,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M454"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A440" zoomScale="188" workbookViewId="0">
-      <selection activeCell="A445" sqref="A445"/>
+    <sheetView tabSelected="1" topLeftCell="A181" zoomScale="188" workbookViewId="0">
+      <selection activeCell="A189" sqref="A189"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -10917,7 +10914,7 @@
     </row>
     <row r="123" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A123" s="6" t="s">
-        <v>2173</v>
+        <v>2172</v>
       </c>
       <c r="B123" s="7" t="s">
         <v>324</v>
@@ -12129,7 +12126,7 @@
     </row>
     <row r="162" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A162" s="12" t="s">
-        <v>2174</v>
+        <v>2173</v>
       </c>
       <c r="B162" s="13" t="s">
         <v>1425</v>
@@ -18263,8 +18260,8 @@
       <c r="C361" s="5" t="s">
         <v>558</v>
       </c>
-      <c r="D361" t="s">
-        <v>2086</v>
+      <c r="D361">
+        <v>909069</v>
       </c>
       <c r="E361" s="3" t="s">
         <v>1019</v>
@@ -18296,7 +18293,7 @@
         <v>311</v>
       </c>
       <c r="D362" t="s">
-        <v>2087</v>
+        <v>2086</v>
       </c>
       <c r="E362" s="19" t="s">
         <v>1020</v>
@@ -18324,7 +18321,7 @@
         <v>1286</v>
       </c>
       <c r="D363" t="s">
-        <v>2088</v>
+        <v>2087</v>
       </c>
       <c r="E363" s="15" t="s">
         <v>1021</v>
@@ -18354,7 +18351,7 @@
         <v>560</v>
       </c>
       <c r="D364" t="s">
-        <v>2089</v>
+        <v>2088</v>
       </c>
       <c r="E364" s="3" t="s">
         <v>1022</v>
@@ -18386,7 +18383,7 @@
         <v>1289</v>
       </c>
       <c r="D365" t="s">
-        <v>2090</v>
+        <v>2089</v>
       </c>
       <c r="E365" s="15" t="s">
         <v>1023</v>
@@ -18416,7 +18413,7 @@
         <v>561</v>
       </c>
       <c r="D366" t="s">
-        <v>2091</v>
+        <v>2090</v>
       </c>
       <c r="E366" s="3" t="s">
         <v>1024</v>
@@ -18448,7 +18445,7 @@
         <v>1292</v>
       </c>
       <c r="D367" t="s">
-        <v>2092</v>
+        <v>2091</v>
       </c>
       <c r="E367" s="15" t="s">
         <v>1025</v>
@@ -18478,7 +18475,7 @@
         <v>562</v>
       </c>
       <c r="D368" t="s">
-        <v>2093</v>
+        <v>2092</v>
       </c>
       <c r="E368" s="3" t="s">
         <v>1026</v>
@@ -18510,7 +18507,7 @@
         <v>313</v>
       </c>
       <c r="D369" t="s">
-        <v>2094</v>
+        <v>2093</v>
       </c>
       <c r="E369" s="19" t="s">
         <v>1027</v>
@@ -18538,7 +18535,7 @@
         <v>1296</v>
       </c>
       <c r="D370" t="s">
-        <v>2095</v>
+        <v>2094</v>
       </c>
       <c r="E370" s="15" t="s">
         <v>1028</v>
@@ -18568,7 +18565,7 @@
         <v>563</v>
       </c>
       <c r="D371" t="s">
-        <v>2096</v>
+        <v>2095</v>
       </c>
       <c r="E371" s="3" t="s">
         <v>1029</v>
@@ -18600,7 +18597,7 @@
         <v>564</v>
       </c>
       <c r="D372" t="s">
-        <v>2097</v>
+        <v>2096</v>
       </c>
       <c r="E372" s="3" t="s">
         <v>1030</v>
@@ -18632,7 +18629,7 @@
         <v>1300</v>
       </c>
       <c r="D373" t="s">
-        <v>2098</v>
+        <v>2097</v>
       </c>
       <c r="E373" s="15" t="s">
         <v>1031</v>
@@ -18662,7 +18659,7 @@
         <v>565</v>
       </c>
       <c r="D374" t="s">
-        <v>2099</v>
+        <v>2098</v>
       </c>
       <c r="E374" s="3" t="s">
         <v>1032</v>
@@ -18694,7 +18691,7 @@
         <v>1303</v>
       </c>
       <c r="D375" t="s">
-        <v>2100</v>
+        <v>2099</v>
       </c>
       <c r="E375" s="15" t="s">
         <v>1033</v>
@@ -18724,7 +18721,7 @@
         <v>566</v>
       </c>
       <c r="D376" t="s">
-        <v>2101</v>
+        <v>2100</v>
       </c>
       <c r="E376" s="3" t="s">
         <v>1034</v>
@@ -18756,7 +18753,7 @@
         <v>317</v>
       </c>
       <c r="D377" t="s">
-        <v>2102</v>
+        <v>2101</v>
       </c>
       <c r="E377" s="19" t="s">
         <v>1035</v>
@@ -18784,7 +18781,7 @@
         <v>1306</v>
       </c>
       <c r="D378" t="s">
-        <v>2103</v>
+        <v>2102</v>
       </c>
       <c r="E378" s="15" t="s">
         <v>1036</v>
@@ -18814,7 +18811,7 @@
         <v>567</v>
       </c>
       <c r="D379" t="s">
-        <v>2104</v>
+        <v>2103</v>
       </c>
       <c r="E379" s="3" t="s">
         <v>1037</v>
@@ -18846,7 +18843,7 @@
         <v>575</v>
       </c>
       <c r="D380" t="s">
-        <v>2105</v>
+        <v>2104</v>
       </c>
       <c r="E380" s="16" t="s">
         <v>1038</v>
@@ -18872,7 +18869,7 @@
         <v>323</v>
       </c>
       <c r="D381" t="s">
-        <v>2106</v>
+        <v>2105</v>
       </c>
       <c r="E381" s="19" t="s">
         <v>1039</v>
@@ -18900,7 +18897,7 @@
         <v>576</v>
       </c>
       <c r="D382" t="s">
-        <v>2107</v>
+        <v>2106</v>
       </c>
       <c r="E382" s="15" t="s">
         <v>1040</v>
@@ -18930,7 +18927,7 @@
         <v>569</v>
       </c>
       <c r="D383" t="s">
-        <v>2108</v>
+        <v>2107</v>
       </c>
       <c r="E383" s="3" t="s">
         <v>1041</v>
@@ -18962,7 +18959,7 @@
         <v>570</v>
       </c>
       <c r="D384" t="s">
-        <v>2109</v>
+        <v>2108</v>
       </c>
       <c r="E384" s="3" t="s">
         <v>1042</v>
@@ -18994,7 +18991,7 @@
         <v>329</v>
       </c>
       <c r="D385" t="s">
-        <v>2110</v>
+        <v>2109</v>
       </c>
       <c r="E385" s="19" t="s">
         <v>1043</v>
@@ -19022,7 +19019,7 @@
         <v>579</v>
       </c>
       <c r="D386" t="s">
-        <v>2111</v>
+        <v>2110</v>
       </c>
       <c r="E386" s="15" t="s">
         <v>1044</v>
@@ -19052,7 +19049,7 @@
         <v>571</v>
       </c>
       <c r="D387" t="s">
-        <v>2112</v>
+        <v>2111</v>
       </c>
       <c r="E387" s="3" t="s">
         <v>1045</v>
@@ -19084,7 +19081,7 @@
         <v>332</v>
       </c>
       <c r="D388" t="s">
-        <v>2113</v>
+        <v>2112</v>
       </c>
       <c r="E388" s="19" t="s">
         <v>1046</v>
@@ -19112,7 +19109,7 @@
         <v>581</v>
       </c>
       <c r="D389" t="s">
-        <v>2114</v>
+        <v>2113</v>
       </c>
       <c r="E389" s="15" t="s">
         <v>1047</v>
@@ -19142,7 +19139,7 @@
         <v>572</v>
       </c>
       <c r="D390" t="s">
-        <v>2115</v>
+        <v>2114</v>
       </c>
       <c r="E390" s="3" t="s">
         <v>1048</v>
@@ -19174,7 +19171,7 @@
         <v>335</v>
       </c>
       <c r="D391" t="s">
-        <v>2116</v>
+        <v>2115</v>
       </c>
       <c r="E391" s="19" t="s">
         <v>1049</v>
@@ -19202,7 +19199,7 @@
         <v>583</v>
       </c>
       <c r="D392" t="s">
-        <v>2117</v>
+        <v>2116</v>
       </c>
       <c r="E392" s="15" t="s">
         <v>1050</v>
@@ -19232,7 +19229,7 @@
         <v>573</v>
       </c>
       <c r="D393" t="s">
-        <v>2118</v>
+        <v>2117</v>
       </c>
       <c r="E393" s="3" t="s">
         <v>1051</v>
@@ -19264,7 +19261,7 @@
         <v>338</v>
       </c>
       <c r="D394" t="s">
-        <v>2119</v>
+        <v>2118</v>
       </c>
       <c r="E394" s="19" t="s">
         <v>1052</v>
@@ -19292,7 +19289,7 @@
         <v>585</v>
       </c>
       <c r="D395" t="s">
-        <v>2120</v>
+        <v>2119</v>
       </c>
       <c r="E395" s="15" t="s">
         <v>1053</v>
@@ -19322,7 +19319,7 @@
         <v>574</v>
       </c>
       <c r="D396" t="s">
-        <v>2121</v>
+        <v>2120</v>
       </c>
       <c r="E396" s="3" t="s">
         <v>1054</v>
@@ -19354,7 +19351,7 @@
         <v>577</v>
       </c>
       <c r="D397" t="s">
-        <v>2122</v>
+        <v>2121</v>
       </c>
       <c r="E397" s="3" t="s">
         <v>1055</v>
@@ -19386,7 +19383,7 @@
         <v>588</v>
       </c>
       <c r="D398" t="s">
-        <v>2123</v>
+        <v>2122</v>
       </c>
       <c r="E398" s="16" t="s">
         <v>1056</v>
@@ -19412,7 +19409,7 @@
         <v>356</v>
       </c>
       <c r="D399" t="s">
-        <v>2124</v>
+        <v>2123</v>
       </c>
       <c r="E399" s="19" t="s">
         <v>1057</v>
@@ -19440,7 +19437,7 @@
         <v>589</v>
       </c>
       <c r="D400" t="s">
-        <v>2125</v>
+        <v>2124</v>
       </c>
       <c r="E400" s="15" t="s">
         <v>1058</v>
@@ -19470,7 +19467,7 @@
         <v>578</v>
       </c>
       <c r="D401" t="s">
-        <v>2126</v>
+        <v>2125</v>
       </c>
       <c r="E401" s="3" t="s">
         <v>1059</v>
@@ -19502,7 +19499,7 @@
         <v>580</v>
       </c>
       <c r="D402" t="s">
-        <v>2127</v>
+        <v>2126</v>
       </c>
       <c r="E402" s="3" t="s">
         <v>1060</v>
@@ -19534,7 +19531,7 @@
         <v>582</v>
       </c>
       <c r="D403" t="s">
-        <v>2128</v>
+        <v>2127</v>
       </c>
       <c r="E403" s="3" t="s">
         <v>1061</v>
@@ -19566,7 +19563,7 @@
         <v>584</v>
       </c>
       <c r="D404" t="s">
-        <v>2129</v>
+        <v>2128</v>
       </c>
       <c r="E404" s="3" t="s">
         <v>1062</v>
@@ -19598,7 +19595,7 @@
         <v>586</v>
       </c>
       <c r="D405" t="s">
-        <v>2130</v>
+        <v>2129</v>
       </c>
       <c r="E405" s="3" t="s">
         <v>1063</v>
@@ -19630,7 +19627,7 @@
         <v>587</v>
       </c>
       <c r="D406" t="s">
-        <v>2131</v>
+        <v>2130</v>
       </c>
       <c r="E406" s="3" t="s">
         <v>1064</v>
@@ -19662,7 +19659,7 @@
         <v>590</v>
       </c>
       <c r="D407" t="s">
-        <v>2132</v>
+        <v>2131</v>
       </c>
       <c r="E407" s="3" t="s">
         <v>1065</v>
@@ -19694,7 +19691,7 @@
         <v>358</v>
       </c>
       <c r="D408" t="s">
-        <v>2133</v>
+        <v>2132</v>
       </c>
       <c r="E408" s="19" t="s">
         <v>1066</v>
@@ -19722,7 +19719,7 @@
         <v>598</v>
       </c>
       <c r="D409" t="s">
-        <v>2134</v>
+        <v>2133</v>
       </c>
       <c r="E409" s="15" t="s">
         <v>1067</v>
@@ -19752,7 +19749,7 @@
         <v>591</v>
       </c>
       <c r="D410" t="s">
-        <v>2135</v>
+        <v>2134</v>
       </c>
       <c r="E410" s="3" t="s">
         <v>1068</v>
@@ -19784,7 +19781,7 @@
         <v>600</v>
       </c>
       <c r="D411" t="s">
-        <v>2136</v>
+        <v>2135</v>
       </c>
       <c r="E411" s="16" t="s">
         <v>1069</v>
@@ -19810,7 +19807,7 @@
         <v>375</v>
       </c>
       <c r="D412" t="s">
-        <v>2137</v>
+        <v>2136</v>
       </c>
       <c r="E412" s="19" t="s">
         <v>1070</v>
@@ -19838,7 +19835,7 @@
         <v>1335</v>
       </c>
       <c r="D413" t="s">
-        <v>2138</v>
+        <v>2137</v>
       </c>
       <c r="E413" s="15" t="s">
         <v>1071</v>
@@ -19868,7 +19865,7 @@
         <v>592</v>
       </c>
       <c r="D414" t="s">
-        <v>2139</v>
+        <v>2138</v>
       </c>
       <c r="E414" s="3" t="s">
         <v>1072</v>
@@ -19900,7 +19897,7 @@
         <v>1337</v>
       </c>
       <c r="D415" t="s">
-        <v>2140</v>
+        <v>2139</v>
       </c>
       <c r="E415" s="16" t="s">
         <v>1073</v>
@@ -19926,7 +19923,7 @@
         <v>394</v>
       </c>
       <c r="D416" t="s">
-        <v>2141</v>
+        <v>2140</v>
       </c>
       <c r="E416" s="19" t="s">
         <v>1074</v>
@@ -19954,7 +19951,7 @@
         <v>1340</v>
       </c>
       <c r="D417" t="s">
-        <v>2142</v>
+        <v>2141</v>
       </c>
       <c r="E417" s="15" t="s">
         <v>1075</v>
@@ -19984,7 +19981,7 @@
         <v>593</v>
       </c>
       <c r="D418" t="s">
-        <v>2143</v>
+        <v>2142</v>
       </c>
       <c r="E418" s="3" t="s">
         <v>1076</v>
@@ -20016,7 +20013,7 @@
         <v>1342</v>
       </c>
       <c r="D419" t="s">
-        <v>2144</v>
+        <v>2143</v>
       </c>
       <c r="E419" s="15" t="s">
         <v>1077</v>
@@ -20046,7 +20043,7 @@
         <v>594</v>
       </c>
       <c r="D420" t="s">
-        <v>2145</v>
+        <v>2144</v>
       </c>
       <c r="E420" s="3" t="s">
         <v>1078</v>
@@ -20078,7 +20075,7 @@
         <v>595</v>
       </c>
       <c r="D421" t="s">
-        <v>2146</v>
+        <v>2145</v>
       </c>
       <c r="E421" s="3" t="s">
         <v>1079</v>
@@ -20110,7 +20107,7 @@
         <v>596</v>
       </c>
       <c r="D422" t="s">
-        <v>2147</v>
+        <v>2146</v>
       </c>
       <c r="E422" s="3" t="s">
         <v>1080</v>
@@ -20142,7 +20139,7 @@
         <v>597</v>
       </c>
       <c r="D423" t="s">
-        <v>2148</v>
+        <v>2147</v>
       </c>
       <c r="E423" s="3" t="s">
         <v>1081</v>
@@ -20174,7 +20171,7 @@
         <v>599</v>
       </c>
       <c r="D424" t="s">
-        <v>2149</v>
+        <v>2148</v>
       </c>
       <c r="E424" s="3" t="s">
         <v>1082</v>
@@ -20206,7 +20203,7 @@
         <v>601</v>
       </c>
       <c r="D425" t="s">
-        <v>2150</v>
+        <v>2149</v>
       </c>
       <c r="E425" s="3" t="s">
         <v>1083</v>
@@ -20238,7 +20235,7 @@
         <v>602</v>
       </c>
       <c r="D426" t="s">
-        <v>2151</v>
+        <v>2150</v>
       </c>
       <c r="E426" s="3" t="s">
         <v>1084</v>
@@ -20270,7 +20267,7 @@
         <v>603</v>
       </c>
       <c r="D427" t="s">
-        <v>2152</v>
+        <v>2151</v>
       </c>
       <c r="E427" s="3" t="s">
         <v>1085</v>
@@ -20302,7 +20299,7 @@
         <v>604</v>
       </c>
       <c r="D428" t="s">
-        <v>2153</v>
+        <v>2152</v>
       </c>
       <c r="E428" s="3" t="s">
         <v>1086</v>
@@ -20334,7 +20331,7 @@
         <v>605</v>
       </c>
       <c r="D429" t="s">
-        <v>2154</v>
+        <v>2153</v>
       </c>
       <c r="E429" s="3" t="s">
         <v>1087</v>
@@ -20366,7 +20363,7 @@
         <v>606</v>
       </c>
       <c r="D430" t="s">
-        <v>2155</v>
+        <v>2154</v>
       </c>
       <c r="E430" s="3" t="s">
         <v>1088</v>
@@ -20398,7 +20395,7 @@
         <v>607</v>
       </c>
       <c r="D431" t="s">
-        <v>2156</v>
+        <v>2155</v>
       </c>
       <c r="E431" s="3" t="s">
         <v>1089</v>
@@ -20430,7 +20427,7 @@
         <v>1353</v>
       </c>
       <c r="D432" t="s">
-        <v>2157</v>
+        <v>2156</v>
       </c>
       <c r="E432" s="15" t="s">
         <v>1090</v>
@@ -20460,7 +20457,7 @@
         <v>608</v>
       </c>
       <c r="D433" t="s">
-        <v>2158</v>
+        <v>2157</v>
       </c>
       <c r="E433" s="3" t="s">
         <v>1091</v>
@@ -20492,7 +20489,7 @@
         <v>609</v>
       </c>
       <c r="D434" t="s">
-        <v>2159</v>
+        <v>2158</v>
       </c>
       <c r="E434" s="3" t="s">
         <v>1092</v>
@@ -20524,7 +20521,7 @@
         <v>397</v>
       </c>
       <c r="D435" t="s">
-        <v>2160</v>
+        <v>2159</v>
       </c>
       <c r="E435" s="19" t="s">
         <v>1093</v>
@@ -20552,7 +20549,7 @@
         <v>1358</v>
       </c>
       <c r="D436" t="s">
-        <v>2161</v>
+        <v>2160</v>
       </c>
       <c r="E436" s="15" t="s">
         <v>1094</v>
@@ -20582,7 +20579,7 @@
         <v>610</v>
       </c>
       <c r="D437" t="s">
-        <v>2162</v>
+        <v>2161</v>
       </c>
       <c r="E437" s="3" t="s">
         <v>1095</v>
@@ -20614,7 +20611,7 @@
         <v>1360</v>
       </c>
       <c r="D438" t="s">
-        <v>2163</v>
+        <v>2162</v>
       </c>
       <c r="E438" s="15" t="s">
         <v>1096</v>
@@ -20644,7 +20641,7 @@
         <v>611</v>
       </c>
       <c r="D439" t="s">
-        <v>2164</v>
+        <v>2163</v>
       </c>
       <c r="E439" s="3" t="s">
         <v>1097</v>
@@ -20676,7 +20673,7 @@
         <v>399</v>
       </c>
       <c r="D440" t="s">
-        <v>2165</v>
+        <v>2164</v>
       </c>
       <c r="E440" s="19" t="s">
         <v>1098</v>
@@ -20704,7 +20701,7 @@
         <v>1363</v>
       </c>
       <c r="D441" t="s">
-        <v>2166</v>
+        <v>2165</v>
       </c>
       <c r="E441" s="15" t="s">
         <v>1099</v>
@@ -20734,7 +20731,7 @@
         <v>612</v>
       </c>
       <c r="D442" t="s">
-        <v>2167</v>
+        <v>2166</v>
       </c>
       <c r="E442" s="3" t="s">
         <v>1100</v>
@@ -20766,7 +20763,7 @@
         <v>413</v>
       </c>
       <c r="D443" t="s">
-        <v>2168</v>
+        <v>2167</v>
       </c>
       <c r="E443" s="19" t="s">
         <v>1101</v>
@@ -20794,7 +20791,7 @@
         <v>1366</v>
       </c>
       <c r="D444" t="s">
-        <v>2169</v>
+        <v>2168</v>
       </c>
       <c r="E444" s="15" t="s">
         <v>1102</v>
@@ -20824,7 +20821,7 @@
         <v>613</v>
       </c>
       <c r="D445" t="s">
-        <v>2170</v>
+        <v>2169</v>
       </c>
       <c r="E445" s="3" t="s">
         <v>1103</v>
@@ -20856,7 +20853,7 @@
         <v>614</v>
       </c>
       <c r="D446" t="s">
-        <v>2171</v>
+        <v>2170</v>
       </c>
       <c r="E446" s="3" t="s">
         <v>1104</v>
@@ -20888,7 +20885,7 @@
         <v>615</v>
       </c>
       <c r="D447" t="s">
-        <v>2172</v>
+        <v>2171</v>
       </c>
       <c r="E447" s="3" t="s">
         <v>1105</v>
@@ -20960,7 +20957,7 @@
         <v>618</v>
       </c>
       <c r="D450" s="3">
-        <v>808158</v>
+        <v>909158</v>
       </c>
       <c r="E450" s="3" t="s">
         <v>1108</v>

</xml_diff>

<commit_message>
[REPO] Actualización calculo incidencias con factores de encadenamiento
</commit_message>
<xml_diff>
--- a/01_datos_crudos/01_03_inpc_complete_NewVersion.xlsx
+++ b/01_datos_crudos/01_03_inpc_complete_NewVersion.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sam/Documents/GitHub/mcv_inflacion/01_datos_crudos/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jorgejuvenalcamposferreira/Documents/GitHub/mcv_inflacion/01_datos_crudos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9DDDA62-B90B-6A44-A9B4-C802A139B3DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E557E4D5-4093-594E-B7FF-B68150611296}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="980" windowWidth="28800" windowHeight="17020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -7055,8 +7055,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N454"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A126" zoomScale="134" workbookViewId="0">
-      <selection activeCell="B135" sqref="B135"/>
+    <sheetView tabSelected="1" zoomScale="134" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7118,6 +7118,9 @@
       <c r="A2" t="s">
         <v>10</v>
       </c>
+      <c r="B2">
+        <v>1.3609522607803</v>
+      </c>
       <c r="C2" s="5" t="s">
         <v>11</v>
       </c>

</xml_diff>

<commit_message>
[WEBMASTER] Infobites 1q Octubre 2024
</commit_message>
<xml_diff>
--- a/01_datos_crudos/01_03_inpc_complete_NewVersion.xlsx
+++ b/01_datos_crudos/01_03_inpc_complete_NewVersion.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jorgejuvenalcamposferreira/Documents/GitHub/mcv_inflacion/01_datos_crudos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E557E4D5-4093-594E-B7FF-B68150611296}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E17596F-209D-F541-91CB-7FBECB5CB904}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="980" windowWidth="28800" windowHeight="17020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -6567,7 +6567,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -6603,6 +6603,13 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="11">
@@ -6710,7 +6717,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -6756,6 +6763,7 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -7056,7 +7064,7 @@
   <dimension ref="A1:N454"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="134" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7118,7 +7126,7 @@
       <c r="A2" t="s">
         <v>10</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="22">
         <v>1.3609522607803</v>
       </c>
       <c r="C2" s="5" t="s">
@@ -7233,7 +7241,7 @@
       <c r="A6" t="s">
         <v>19</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="23">
         <v>1.52057007048839</v>
       </c>
       <c r="C6" s="5" t="s">

</xml_diff>